<commit_message>
Week-04 R solution added
</commit_message>
<xml_diff>
--- a/week-04/Model Representation.xlsx
+++ b/week-04/Model Representation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26000" windowHeight="16500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26840" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Zero Hidden Layear" sheetId="1" r:id="rId1"/>
@@ -347,36 +347,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -456,20 +456,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>186170</xdr:rowOff>
+      <xdr:rowOff>96119</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPr id="3" name="Рисунок 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -482,8 +482,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1739900" y="2692400"/>
-          <a:ext cx="5372100" cy="2319770"/>
+          <a:off x="1536700" y="2743200"/>
+          <a:ext cx="5003800" cy="2178919"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -819,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,44 +834,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="16"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="7"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="16"/>
       <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="26" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="3"/>
@@ -880,93 +880,93 @@
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="11">
+      <c r="A4" s="9">
         <v>0</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>0</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>30</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="9">
         <v>-20</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <v>-20</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="11">
         <f>$D$4+$E$4*A4+$F$4*B4</f>
         <v>30</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="12">
         <f>1/(1+EXP(-H4))</f>
         <v>0.99999999999990652</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="11">
-        <v>1</v>
-      </c>
-      <c r="B5" s="11">
+      <c r="A5" s="9">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9">
         <v>0</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="11">
         <f t="shared" ref="H5:H7" si="0">$D$4+$E$4*A5+$F$4*B5</f>
         <v>10</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="12">
         <f>1/(1+EXP(-H5))</f>
         <v>0.99995460213129761</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="11">
-        <v>1</v>
-      </c>
-      <c r="B6" s="11">
-        <v>1</v>
-      </c>
-      <c r="H6" s="13">
+      <c r="A6" s="9">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="11">
         <f t="shared" si="0"/>
         <v>-10</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="12">
         <f>1/(1+EXP(-H6))</f>
         <v>4.5397868702434395E-5</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="11">
+      <c r="A7" s="9">
         <v>0</v>
       </c>
-      <c r="B7" s="11">
-        <v>1</v>
-      </c>
-      <c r="H7" s="13">
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="H7" s="11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="12">
         <f>1/(1+EXP(-H7))</f>
         <v>0.99995460213129761</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="1"/>
@@ -974,10 +974,10 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1011,58 +1011,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="L1" s="10" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="L1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
     </row>
     <row r="2" spans="1:16" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="7"/>
+      <c r="J2" s="16"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
       <c r="O2" s="6"/>
       <c r="P2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -1078,10 +1078,10 @@
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:16" ht="28" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="3"/>
@@ -1090,10 +1090,10 @@
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="18"/>
+      <c r="H4" s="17"/>
       <c r="I4" s="15" t="s">
         <v>16</v>
       </c>
@@ -1104,199 +1104,194 @@
       </c>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="P4" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="16">
+      <c r="A5" s="13">
         <v>0</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="13">
         <v>0</v>
       </c>
-      <c r="D5" s="11">
-        <v>30</v>
-      </c>
-      <c r="E5" s="11">
-        <v>10</v>
-      </c>
-      <c r="F5" s="11">
-        <v>-60</v>
-      </c>
-      <c r="G5" s="13">
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F5" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G5" s="11">
         <f>$D$5+$E$5*A5+$F$5*B5</f>
-        <v>30</v>
-      </c>
-      <c r="H5" s="13">
+        <v>1</v>
+      </c>
+      <c r="H5" s="11">
         <f>$D$6+$E$6*A5+$F$6*B5</f>
-        <v>-30</v>
-      </c>
-      <c r="I5" s="13">
+        <v>1</v>
+      </c>
+      <c r="I5" s="11">
         <f>1/(1+EXP(-G5))</f>
-        <v>0.99999999999990652</v>
-      </c>
-      <c r="J5" s="14">
+        <v>0.7310585786300049</v>
+      </c>
+      <c r="J5" s="12">
         <f>1/(1+EXP(-H5))</f>
-        <v>9.3576229688392989E-14</v>
-      </c>
-      <c r="L5" s="11">
-        <v>10</v>
-      </c>
-      <c r="M5" s="11">
-        <v>-30</v>
-      </c>
-      <c r="N5" s="12">
-        <v>20</v>
-      </c>
-      <c r="O5" s="14">
+        <v>0.7310585786300049</v>
+      </c>
+      <c r="L5" s="9">
+        <v>1</v>
+      </c>
+      <c r="M5" s="9">
+        <v>-0.8</v>
+      </c>
+      <c r="N5" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="O5" s="12">
         <f>$L$5+$M$5*I5+$N$5*J5</f>
-        <v>-19.999999999995325</v>
-      </c>
-      <c r="P5" s="14">
+        <v>0.853788284273999</v>
+      </c>
+      <c r="P5" s="12">
         <f>1/(1+EXP(-O5))</f>
-        <v>2.0611536181998404E-9</v>
+        <v>0.70136121726231537</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="16">
-        <v>1</v>
-      </c>
-      <c r="B6" s="16">
+      <c r="A6" s="13">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13">
         <v>0</v>
       </c>
-      <c r="D6" s="11">
-        <v>-30</v>
-      </c>
-      <c r="E6" s="11">
-        <v>20</v>
-      </c>
-      <c r="F6" s="11">
-        <v>10</v>
-      </c>
-      <c r="G6" s="13">
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
+        <v>-1.5</v>
+      </c>
+      <c r="F6" s="9">
+        <v>3.7</v>
+      </c>
+      <c r="G6" s="11">
         <f t="shared" ref="G6:G8" si="0">$D$5+$E$5*A6+$F$5*B6</f>
-        <v>40</v>
-      </c>
-      <c r="H6" s="13">
+        <v>6.1</v>
+      </c>
+      <c r="H6" s="11">
         <f t="shared" ref="H6:H8" si="1">$D$6+$E$6*A6+$F$6*B6</f>
-        <v>-10</v>
-      </c>
-      <c r="I6" s="13">
+        <v>-0.5</v>
+      </c>
+      <c r="I6" s="11">
         <f t="shared" ref="I6:I8" si="2">1/(1+EXP(-G6))</f>
-        <v>1</v>
-      </c>
-      <c r="J6" s="14">
+        <v>0.9977621514787236</v>
+      </c>
+      <c r="J6" s="12">
         <f t="shared" ref="J6:J8" si="3">1/(1+EXP(-H6))</f>
-        <v>4.5397868702434395E-5</v>
-      </c>
-      <c r="O6" s="14">
+        <v>0.37754066879814541</v>
+      </c>
+      <c r="O6" s="12">
         <f t="shared" ref="O6:O8" si="4">$L$5+$M$5*I6+$N$5*J6</f>
-        <v>-19.99909204262595</v>
-      </c>
-      <c r="P6" s="14">
+        <v>0.42831468009590828</v>
+      </c>
+      <c r="P6" s="12">
         <f t="shared" ref="P6:P8" si="5">1/(1+EXP(-O6))</f>
-        <v>2.0630259076639214E-9</v>
+        <v>0.60547115787525618</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="16">
-        <v>1</v>
-      </c>
-      <c r="B7" s="16">
-        <v>1</v>
-      </c>
-      <c r="G7" s="13">
+      <c r="A7" s="13">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11">
         <f t="shared" si="0"/>
-        <v>-20</v>
-      </c>
-      <c r="H7" s="13">
+        <v>8.3999999999999986</v>
+      </c>
+      <c r="H7" s="11">
         <f t="shared" si="1"/>
+        <v>3.2</v>
+      </c>
+      <c r="I7" s="11">
+        <f t="shared" si="2"/>
+        <v>0.99977518322976666</v>
+      </c>
+      <c r="J7" s="12">
+        <f t="shared" si="3"/>
+        <v>0.96083427720323566</v>
+      </c>
+      <c r="O7" s="12">
+        <f t="shared" si="4"/>
+        <v>0.77668041973812796</v>
+      </c>
+      <c r="P7" s="12">
+        <f t="shared" si="5"/>
+        <v>0.68496422778853916</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
         <v>0</v>
       </c>
-      <c r="I7" s="13">
+      <c r="B8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" si="0"/>
+        <v>3.3</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" si="1"/>
+        <v>4.7</v>
+      </c>
+      <c r="I8" s="11">
         <f t="shared" si="2"/>
-        <v>2.0611536181902037E-9</v>
-      </c>
-      <c r="J7" s="14">
+        <v>0.96442881072736386</v>
+      </c>
+      <c r="J8" s="12">
         <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="O7" s="14">
+        <v>0.99098670134715205</v>
+      </c>
+      <c r="O8" s="12">
         <f t="shared" si="4"/>
-        <v>19.999999938165391</v>
-      </c>
-      <c r="P7" s="14">
+        <v>0.82304897222640006</v>
+      </c>
+      <c r="P8" s="12">
         <f t="shared" si="5"/>
-        <v>0.99999999793884631</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="16">
-        <v>0</v>
-      </c>
-      <c r="B8" s="16">
-        <v>1</v>
-      </c>
-      <c r="G8" s="13">
-        <f t="shared" si="0"/>
-        <v>-30</v>
-      </c>
-      <c r="H8" s="13">
-        <f t="shared" si="1"/>
-        <v>-20</v>
-      </c>
-      <c r="I8" s="13">
-        <f t="shared" si="2"/>
-        <v>9.3576229688392989E-14</v>
-      </c>
-      <c r="J8" s="14">
-        <f t="shared" si="3"/>
-        <v>2.0611536181902037E-9</v>
-      </c>
-      <c r="O8" s="14">
-        <f t="shared" si="4"/>
-        <v>10.000000041220266</v>
-      </c>
-      <c r="P8" s="14">
-        <f t="shared" si="5"/>
-        <v>0.99995460213316878</v>
+        <v>0.69488316871826661</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13" t="s">
+      <c r="H9" s="11"/>
+      <c r="I9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="14" t="s">
+      <c r="O9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="P9" s="14" t="s">
+      <c r="P9" s="12" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="L4:N4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="A2:B2"/>
@@ -1304,6 +1299,11 @@
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="L4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>